<commit_message>
added QA for export. found & fixed date bug (error: input: 09/14/2025, output 09/13/2025)
</commit_message>
<xml_diff>
--- a/backend/Payroll Copy - AscentUP.xlsx
+++ b/backend/Payroll Copy - AscentUP.xlsx
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,22 +506,22 @@
         <v>b@gmail.com</v>
       </c>
       <c r="B5">
-        <v>18.5</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="str">
-        <v>California</v>
+        <v>Georgia</v>
       </c>
       <c r="E5" t="str">
-        <v>Client 1</v>
+        <v>Acme</v>
       </c>
       <c r="F5" t="str">
         <v>09/13–09/26</v>
       </c>
       <c r="G5" t="str">
-        <v/>
+        <v>Consult #1</v>
       </c>
     </row>
     <row r="6">
@@ -547,9 +547,32 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>b@gmail.com</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Georgia</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Acme</v>
+      </c>
+      <c r="F7" t="str">
+        <v>09/14–09/27</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Special Consult #2</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>